<commit_message>
new update and new jpnb
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shannon.cap\Documents\GitHub\sistematizacion_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD8B49A-0A13-4652-9F4E-E07C8536FD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F40F08-24E8-42C4-BF10-D9A24507ACF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="735" windowWidth="15435" windowHeight="15465" xr2:uid="{F46115C4-AD7F-4302-BE6E-0AA369B82E4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F46115C4-AD7F-4302-BE6E-0AA369B82E4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="180">
   <si>
     <t>Sector</t>
   </si>
@@ -80,18 +81,12 @@
     <t>Hay que partir, ya que, por parte de la cooperación internacional, puesto que de esta parte ya se cuenta con la colaboración, y lograr los contactos necesarios, poder evaluar a nivel global y no solo lo regional y facilitar el conocimiento.</t>
   </si>
   <si>
-    <t>Recordar que todos los esfuerzos deben centrarse en las personas y no olvidar a los grupos vulnerables, es decir mujeres, niños, comunidades indiginas, es decir que nadie se quede atrás.</t>
-  </si>
-  <si>
     <t>Una ley especifica de ciberseguridad es muy importante, a pesar de que un marco de ley sea amplio, de protección, es necesario tener una ley especifica de ciberseguridad. Es un tema de alta prioridad porque por ejemplo tener un ciberataque en infraestructuras publicas seria letal, ya que la ciberdelincuencia no tiene fronteras, ya que, en alguna oportunidad en dos o tres gobiernos, existió una estrategia nacional de ciberseguridad que se trabajo conjunto a la OEA.</t>
   </si>
   <si>
     <t>La cooperación podrá apoyar con las investigaciones académicas, para que tengan una preparación más fuerte.</t>
   </si>
   <si>
-    <t>La importancia de saber manejar los contenidos, pues de que serviría que la gente logre adquirir internet, si solo se utiliza en contenido sin provecho, tendría que ser al contrario, seria bueno saber como llevar la afabetizacion digital para que la gente saque provecho de esta digitalización. Y saber si el sector privado sea tan interesante o invertir en las comunidades, puesto que en materia de negocio seria bueno investigar eso.</t>
-  </si>
-  <si>
     <t>Es importante fortalecer a los cuerpos de seguridad, y crear condiciones de infraestructura digital, se necesita mucho y en términos de la misma lógica del proceso de modernización, el tema de capital humano, es bueno pensar en que tipo de perfil profesional sería necesarios para abordar las necesidades.</t>
   </si>
   <si>
@@ -131,9 +126,6 @@
     <t>Exigir la actualización de datos y desde allí se pueda dar la ciberseguridad</t>
   </si>
   <si>
-    <t xml:space="preserve">Liberta de expresión </t>
-  </si>
-  <si>
     <t>Tener insumos de lo que se necesita, al final las sociedades civiles somos los beneficiarios, tener a la vista las decisiones de políticas publicas relacionada a la ciberseguridad.</t>
   </si>
   <si>
@@ -206,69 +198,9 @@
     <t>Concientizar y sensibilizar sobre la importancia de ciberseguridad</t>
   </si>
   <si>
-    <t>Implementar el acceso a la electricididad, equipo tecnologico e internet en los departamentos del interior del pais.</t>
-  </si>
-  <si>
-    <t>Como estudiantes podriamos contribuir en la formaciòn de ciberseguridad. (concienciaciòns, infografias, capacitaciones, entre otros.)</t>
-  </si>
-  <si>
-    <t>Llevar estos dialogos a los departamentos del interior del paìs, asimismo, buscar alianzas internacionales, con el objetivo de promover la eduaciòn en temas de ciberseguridad.</t>
-  </si>
-  <si>
-    <t>Implementar un sistema para poder digitalizar la informaciòn, crear bases de datos, fomentar la ciberseguridad y la digitalizaciòn. CCDA.</t>
-  </si>
-  <si>
-    <t>Alianzas del sector pùblico y academicos para contribuir a la educaciòn en temas de ciberseguridad, permitiendo que sen impartido en los diferentes sectores estudiantiles y poblaciòn en general.</t>
-  </si>
-  <si>
-    <t>Proteger los datos de la poblaciòn con el objetivo de ser vìctimas de algun tipo de delito. Ademàs, abrir màs espacios las comunidades rurales e indigenas con el fin de expandir dichos temas.</t>
-  </si>
-  <si>
-    <t>Accesibilidad a la informaciòn, debe de ser transparante el proceso, fomentar e incluir a la poblaciòn.</t>
-  </si>
-  <si>
-    <t>SBX, podrìa contribuir en talleres enfocados a los estudiantes, COCODES, entre otros, en temas de ciberseguridad; resaltando a la poblaciòn de las tercera edad quienes son considerados como los màs vulnerables en dichos temas. Ademàs, buscar apoyo internacional.</t>
-  </si>
-  <si>
-    <t>Transparencia por parte del Gobierno, brindar la informaciòn de lo que se esta trabajando. Trabajar en conjunto con la sociedad civil.</t>
-  </si>
-  <si>
-    <t>Poca de confianza de la poblaciòn en las instituciones.</t>
-  </si>
-  <si>
-    <t>Como sector estudiantil, podrìa contribuir en la difusiòn de temas relacionados a la ciberseguridad.</t>
-  </si>
-  <si>
     <t>Impulsar las iniciativas de ley ya propuestas de ciberseguridad.</t>
   </si>
   <si>
-    <t>Acceso al internet, fomentaciòn a la participaciòn de los jovenes, incentivar la ciberseguridad en todos los niveles. Ademàs, la creaciòn de plataformas seguras en el sector academico.</t>
-  </si>
-  <si>
-    <t>Crear contenido a traves de las redes sociales y campañas radiales para alcanzar a todas la comunidades y promover la educaciòn en temas de ciberseguridad.</t>
-  </si>
-  <si>
-    <t>Crear platafomas seguras para proteger los datos personales de la poblaciòn; ademàs, trabajar en conjunto con el sector privado.</t>
-  </si>
-  <si>
-    <t>Realizar anàlisis de riesgos en temas de ciberseguridad. (como sociedad civil).</t>
-  </si>
-  <si>
-    <t>Articulando organizaciones en los distintos departamentos donde el acceso a los servicios basicos es limitado, para colaborar en la fomentaciòn de la ciberseguridad mediante el apoyo de las instituciones pùblicas y privadas.</t>
-  </si>
-  <si>
-    <t>Incentivar los conversatorios o talleres a nivel nacional, incluyendo a los distintos sectores, con el objetivo de promover la educaciòn en ciberseguridad; asimismo, desarrollar ejercicios pràcticos.</t>
-  </si>
-  <si>
-    <t>Formaciòn en temas de ciberseguridad en todos los niveles y que sea impartido en los distintos idiomas, con el objetivo de llegar a todas la comunidades.</t>
-  </si>
-  <si>
-    <t>Promover y apoyar en la educaciòn de la ciberseguridad a las alcaldias auxiliares, para expandir temas relacionados a la ciberseguridad.</t>
-  </si>
-  <si>
-    <t>Que el Gobierno sea transparente y que brinde informaciòn sobre a quienes se les esta brindando los datos personales, con el objetivo de que la poblaciòn tenga confianza.</t>
-  </si>
-  <si>
     <t>Implementar temas educativos, como conferencias de ciberseguridad, tomar en cuenta que todos deben ser capacitados, porque desde un niño que usa un celular ya debería saber de ciberseguridad, porque se debe tomar en cuenta que si esta conectado, esta expuesto.</t>
   </si>
   <si>
@@ -308,7 +240,372 @@
     <t>P3</t>
   </si>
   <si>
-    <t>Uno de los temas a considerar, sería la creación de un marco legal, ya que no puede esperar más el tema de ciberseguridad. Ya que da soporte, y estrategias para accionar, incluyendo el tema normativo, es importante como se va aplicar, la inclusión de un reglamento y los procedimientos, ya que el convenio de BUDAPEST es prioridad para poder adherirse, y poder participar de verdad dentro del intercambio.</t>
+    <t>Sector Privado</t>
+  </si>
+  <si>
+    <t>Uno de los temas a considerar, sería la creación de un MARCO LEGAL, ya que no puede esperar más el tema de ciberseguridad. Ya que da soporte, y estrategias para accionar, incluyendo el tema normativo, es importante como se va aplicar, la inclusión de un reglamento y los procedimientos, ya que el convenio de BUDAPEST es prioridad para poder adherirse, y poder participar de verdad dentro del intercambio.</t>
+  </si>
+  <si>
+    <t>Recordar que todos los esfuerzos deben centrarse en las personas y no olvidar a los grupos vulnerables, es decir mujeres, niños, comunidades indígenas, es decir que nadie se quede atrás.</t>
+  </si>
+  <si>
+    <t>La importancia de saber manejar los contenidos, pues de que serviría que la gente logre adquirir internet, si solo se utiliza en contenido sin provecho, tendría que ser al contrario, seria bueno saber como llevar la alfabetización digital para que la gente saque provecho de esta digitalización. Y saber si el sector privado sea tan interesante o invertir en las comunidades, puesto que en materia de negocio seria bueno investigar eso.</t>
+  </si>
+  <si>
+    <t>Implementar el acceso a la electricidad, equipo tecnológico e internet en los departamentos del interior del país.</t>
+  </si>
+  <si>
+    <t>Como estudiantes podríamos contribuir en la formación de ciberseguridad. (concienciación, infografías, capacitaciones, entre otros.)</t>
+  </si>
+  <si>
+    <t>Llevar estos diálogos a los departamentos del interior del país, asimismo, buscar alianzas internacionales, con el objetivo de promover la educación en temas de ciberseguridad.</t>
+  </si>
+  <si>
+    <t>Implementar un sistema para poder digitalizar la información, crear bases de datos, fomentar la ciberseguridad y la digitalización. CCDA.</t>
+  </si>
+  <si>
+    <t>Alianzas del sector público y académicos para contribuir a la educación en temas de ciberseguridad, permitiendo que sen impartido en los diferentes sectores estudiantiles y población en general.</t>
+  </si>
+  <si>
+    <t>Proteger los datos de la población con el objetivo de ser víctimas de algún tipo de delito. Además, abrir más espacios las comunidades rurales e indígenas con el fin de expandir dichos temas.</t>
+  </si>
+  <si>
+    <t>Accesibilidad a la información, debe de ser transparente el proceso, fomentar e incluir a la población.</t>
+  </si>
+  <si>
+    <t>SBX, podría contribuir en talleres enfocados a los estudiantes, COCODES, entre otros, en temas de ciberseguridad; resaltando a la población de las tercera edad quienes son considerados como los más vulnerables en dichos temas. Además, buscar apoyo internacional.</t>
+  </si>
+  <si>
+    <t>Transparencia por parte del Gobierno, brindar la información de lo que se esta trabajando. Trabajar en conjunto con la sociedad civil.</t>
+  </si>
+  <si>
+    <t>Poca de confianza de la población en las instituciones.</t>
+  </si>
+  <si>
+    <t>Como sector estudiantil, podría contribuir en la difusión de temas relacionados a la ciberseguridad.</t>
+  </si>
+  <si>
+    <t>Acceso al internet, fomentación a la participación de los jóvenes, incentivar la ciberseguridad en todos los niveles. Además, la creación de plataformas seguras en el sector académico.</t>
+  </si>
+  <si>
+    <t>Crear contenido a través de las redes sociales y campañas radiales para alcanzar a todas la comunidades y promover la educación en temas de ciberseguridad.</t>
+  </si>
+  <si>
+    <t>Crear plataformas seguras para proteger los datos personales de la población; además, trabajar en conjunto con el sector privado.</t>
+  </si>
+  <si>
+    <t>Realizar análisis de riesgos en temas de ciberseguridad. (como sociedad civil).</t>
+  </si>
+  <si>
+    <t>Articulando organizaciones en los distintos departamentos donde el acceso a los servicios básicos es limitado, para colaborar en la fomentación de la ciberseguridad mediante el apoyo de las instituciones públicas y privadas.</t>
+  </si>
+  <si>
+    <t>Incentivar los conversatorios o talleres a nivel nacional, incluyendo a los distintos sectores, con el objetivo de promover la educación en ciberseguridad; asimismo, desarrollar ejercicios prácticos.</t>
+  </si>
+  <si>
+    <t>Formación en temas de ciberseguridad en todos los niveles y que sea impartido en los distintos idiomas, con el objetivo de llegar a todas la comunidades.</t>
+  </si>
+  <si>
+    <t>Promover y apoyar en la educación de la ciberseguridad a las alcaldías auxiliares, para expandir temas relacionados a la ciberseguridad.</t>
+  </si>
+  <si>
+    <t>Que el Gobierno sea transparente y que brinde información sobre a quienes se les esta brindando los datos personales, con el objetivo de que la población tenga confianza.</t>
+  </si>
+  <si>
+    <t>Libertad de expresión</t>
+  </si>
+  <si>
+    <t>Las prioridades responden a los aportes que desde la academia se puedan realizar para entender las necesidades de país y aportar con investigaciones y datos actualizados</t>
+  </si>
+  <si>
+    <t>Aportando datos y discusiones académicas sobre la transformación digital</t>
+  </si>
+  <si>
+    <t>Las recomendaciones estarán enfocadas en los objetivos que proponga el Gobierno para atender las necesidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vision, hoja de ruta y colaboración. Urgente una Agenda de Transformación Digital de Guatemala </t>
+  </si>
+  <si>
+    <t>Estudios, ideas, mejores prácticas, colaboración con talleres, redes y propuestas concretas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decidir si se necesita una ley marco, definición clara de la estrategia, división del trabajo, actuar y evaluar. Involucrar a todos,inspirar y caminar juntos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Datos abiertos y anticorrupción 
+2. Formación a la sociedad civil sobre temas de gobierno </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Procesos de investigación y asesoría a partir del análisis de datos abiertos para acciones anticorrupción en distintos niveles y sectores. 
+2. Procesos de formación de funcionarios públicos, sociedad civil y sector privado sobre la implementación de gobierno abierto y electrónico. 
+3. Procesos de difusión e incidencia del gobierno abierto a partir de análisis y publicaciones académicas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Continuar con el enfoque participativo y consenso entre sectores 
+2. Tomar buenas prácticas de otros países de la región latinoamericana considerando las particularidades socioculturales compartidas 
+3. Priorizar temas específicos de transformación digital que beneficien a la mayor parte de la población para que pueda generar confianza ciudadana y adopción de los procesos de digitalización 
+4. Emprender acciones de educación y promoción de la transformación digital 
+5. Que el proceso de transformación digital aporte simultáneamente al cierre de la brecha digital 
+</t>
+  </si>
+  <si>
+    <t>Cooperación internacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modernización y facilitación de los servicios, fortalecimiento de las capacidades de las instituciones del sector público, mejora de la calidad de los servicios de educación y salud, desarrollo sostenible e inclusivo, protección del medio ambiente, equidad de género </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A través de la cooperación internacional, intercambio de experiencias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modernización de la tecnología, promover la interoperabilidad, </t>
+  </si>
+  <si>
+    <t>Cuerpo Diplomático</t>
+  </si>
+  <si>
+    <t>Rectoría, identidad digital, base de datos nacional, y respaldo legal, acceso y protocolos para desarrollo de servicios públicos digitales sensibles a la infancia y pueblos originarios. Fortalecimiento de capacidades (currículum actualizado al contexto)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apoyo técnico para la construcción de leyes/protocolos y pilotos. Financiamiento limitado para acciones. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear una hoja de ruta y un abordaje por fases. Priorizando el área legal y la estandarización de tecnologías y procesos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La gobernanza, la alfabetización digital, la inclusión para reducir las brechas digitales existentes como pueblos indígenas y la brecha de género. Es importante empoderar al Estado para que se pueda entender la importancia que tiene la transformación digital en Guatemala </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con apoyo técnico y de creación de habilidades tanto para el gobierno como para la población general en cuanto a temas relacionados a la Alfabetización digital, el uso de la inteligencia artificial y el uso de las tecnologías de manera responsable y segura. Contamos con estudios a nivel global que pueden implementarse en Guatemala </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es importante la creación de un marco legal y de una policía de estado  sostenible en el tiempo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulsar infraestructuras públicas digitales en el país de manera coordinada y articulada. Entre ellas, la interoperabllifad, identidad digital y pagos digitales para tener un salto tecnológico que acelere la prestación de servicios del Estado, asegurando la inclusión digital en este proceso. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cómo socio estratégico que contribuye con conocimiento, acompañamiento técnico y logístico, convocatoria y coordinación de múltiples actores, apoyo de pilotos estratégicos. </t>
+  </si>
+  <si>
+    <t>Alinear los esfuerzo a una única agenda de transformación digital del país. Esto implica colaborar con sector privado, academia, sociedad civil, cooperantes. A través de esta agenda canalizar las necesidades de las instituciones para evitar la fragmentación y uso disperso de tecnologías que dificulten a los usuarios (ciudadanos) el acceso a los servicios digitales. Integrar la experiencia de usuario a los planes digitales de las instituciones y el re diseño de servicios digitales.</t>
+  </si>
+  <si>
+    <t>Las empresas inversoras y exportadoras requieren procesos claros, objetivos, seguros y rápidos o eficientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las empresas españolas de tecnología y consultoras pueden contribuir con su experiencia a aportar soluciones tecnológicas y de gestión </t>
+  </si>
+  <si>
+    <t>Hay que empezar por proyectos piloto que permitan generar soluciones primearias</t>
+  </si>
+  <si>
+    <t>Gobierno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simplificación de trámites y datos abiertos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siguiendo las leyes y acuerdos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voluntad política </t>
+  </si>
+  <si>
+    <t>Privado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simplificación y digitalización de trámites, por lo que la interiperabilidad es fundamental. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desde Guatemala No se detiene se apoya estos estos procesos con consultores y enlaces </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gobernanza, agenda nacional de pais, ejecución de proyectos coordinada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tramites de Registros y Otras gestiones en Control de Alimentos del MSPAS
+Tramites de Alimentos Laboratorio Nacional MSPAS
+Consultas sobre Registros Sanitarios de Alimentosn en Linea.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apoyando estas iniciativas en las mesas de dialogo.
+Proponiendo Ideas para reducir Focos de Corruocion en tramitologia.
+Socializando la iniciativa dentro de su propio sector.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificar los Puntos Criticos de Corrupcion en la tramitologia de Estado para automatizarlos.
+Garantizar el acceso a tramitologia de Estado por medio de APPs para Celulares.
+Mucha Comunicacion Efectiva.
+</t>
+  </si>
+  <si>
+    <t>1. Agilizar y eliminar la discrecionalidad en trámites y registros
+2. Transparentar las compras y adquisiciones del Estado
+3. Haciendo que procesos educativos y de modernización de la sociedad lleguen a más personas y en menos tiempo</t>
+  </si>
+  <si>
+    <t>1. Trasladando capacidades del sector privado hacia el público
+2. Proponiendo metodologías de priorización y seguimiento
+3. Haciendo incidencia política para que las reformas legales e implementación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Establecer ruta, visión de qué significa y hacer comunicación efectiva a toda la sociedad
+2. Priorizar las áreas y procesos que generen mayor impacto en transparencia y servicio a la ciudadanía
+3. Establecer hoja de ruta y empoderar a la GAE para que fije los estándares y exija cuentadancia al resto de dependencias
+4. Socializar metas, logros y alcances </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacer público las APIs a todos los usuarios que lo requiera </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que permita a las Pymes tecnologícas a participar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compras de Gobierno </t>
+  </si>
+  <si>
+    <t>Agilización de tramites de caracter regulatorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tenemos experiencia en simplificación de tramites regulatorios, levantamiento de procesos y agilizsción para hacer ttamites digitales desde 1987. 
+</t>
+  </si>
+  <si>
+    <t>Tramites regulatorios en MSPAS- regustros, licencias, renovación de registros para medicamentos y alimentos. 
+Licencias ambientales MARN.
+Tramites en MAGA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobertura digital </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campañas de información </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobertura digital 
+Campaña de información </t>
+  </si>
+  <si>
+    <t>Identidad Digital e Interoperabilidad de las entidades del Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitación de jóvenes y otros programas de capacitación basados en la comunidad. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinación y unificación de esfuerzos. Trabajo técnico y práctico. Instituciionalidad de los procesos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facilitación de trámites y acceso a la tecnología </t>
+  </si>
+  <si>
+    <t>Aportando nuestras experiencias y perspectivas y procurando la inclusión de nuestro colectivo</t>
+  </si>
+  <si>
+    <t>Que las instituciones sean adecuadamente capacitadas y provistas de los recursos para poder cumplir con su trabajo</t>
+  </si>
+  <si>
+    <t>Recursos para la Educación, diseño de herramientas y uso de medios radiales, etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño de herramientas, formación de formadores a nivel local, estrategias de comunicación para la transparencia </t>
+  </si>
+  <si>
+    <t>Voluntad política, asignación de presupuesto y formación y educación continua</t>
+  </si>
+  <si>
+    <t>La digitalización de la información de las instituciones publicas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aportando a la discusión y creación de políticas de transformación digital </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No dejar por lado a la ciudadanía en la discusión, esta transformación debe servir para mejorar la vida de las y los ciudadanos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Facilitar información a grupos de mujeres en los territorios 2) Fortalecimiento de capacidades  a grupos de mujeres en herramientas digitales en los territorios. 
+</t>
+  </si>
+  <si>
+    <t>Réplicas de conocimientos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incluir a las mujeres en los procesos de transformación digital. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitación continua, una desmonopolizacion del servicio de Internet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informar a las mujeres con quienes trabajamos </t>
+  </si>
+  <si>
+    <t>Internet seguro y rápido, y de ser posible tecnología al alcance de la población.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educación inclusiva </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creando alianzas entre sectores </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lograr operativisar entre organizaciones del ejecutivo o </t>
+  </si>
+  <si>
+    <t>Formación digital, acceso a medios.</t>
+  </si>
+  <si>
+    <t>Llevando información, formación y recursos a comunidades indígenas (48 Cantones)</t>
+  </si>
+  <si>
+    <t>Gobierno electrónico para la eficiencia y eficacia estatal.....</t>
+  </si>
+  <si>
+    <t>Facilitar los procesos y trámites que como jóvenes nos podemos llegar a enfrentar por primera vez.</t>
+  </si>
+  <si>
+    <t>Difusión y capacitación de la población universitaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que sea fácil de entender y ágil </t>
+  </si>
+  <si>
+    <t>Interconectar la información del gobierno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cómo usuarios de los sistemas podemos apoyar en garantizar las necesidades de la ciudadanía, con pertinencia de género, e interculturalidad. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un proceso de comunicación claro para dar a conocer los cambios. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrategia nacional de transformación digital, legislación moderna y fortalecida, espacios de participación, inversión pública, voluntad política </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrategias y capacidades sobre impletacion de la estrategia, conocimiento de necesidades de la población específicamente de grupos poblacionales qué son vulnerables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorporar organizaciónes del interior del país, comunicación constante entre entidades públicas a todo nivel. </t>
+  </si>
+  <si>
+    <t>Trabajo y salario competente que permita adquirir dispositivos tecnológicos y capacitación digital. Además que permita disponer de internet regular.</t>
+  </si>
+  <si>
+    <t>Aportar con validar el contenido y también con socializar el contenido de transformación digital.</t>
+  </si>
+  <si>
+    <t>Que realice un diagnóstico responsable en las comunidades rurales antes de crear contenido, estrategias. El diagnóstico debe a qué tienen acceso las personas en las áreas rurales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contar con herramientas accesibles y fáciles de utilizar. El internet debe ser accesible </t>
+  </si>
+  <si>
+    <t>Validar las herramientas digitales para ser accesibles e informar sobre la transformación digital que se está desarrollando en el Estado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear espacios accesibles para hacer uso de la digitalización del gobierno </t>
   </si>
 </sst>
 </file>
@@ -318,7 +615,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;Q&quot;#,##0;[Red]\-&quot;Q&quot;#,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +635,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -396,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -433,6 +738,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4893CB-7321-44A7-B457-11B87E195EC7}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,13 +1096,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -854,13 +1162,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -868,13 +1176,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -882,13 +1190,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -896,317 +1204,760 @@
         <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="7" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="7" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>24</v>
+      <c r="A20" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D31" s="7"/>
     </row>
+    <row r="33" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB04D74B-203B-4761-8727-6A55601EBBBC}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>